<commit_message>
enhanced fields autocomplete with templates
</commit_message>
<xml_diff>
--- a/backend/resources/Konduga.xlsx
+++ b/backend/resources/Konduga.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,10 +529,8 @@
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -574,10 +572,8 @@
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -619,10 +615,8 @@
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -664,10 +658,8 @@
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -709,10 +701,8 @@
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -754,10 +744,8 @@
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -799,10 +787,8 @@
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -844,10 +830,8 @@
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -889,10 +873,8 @@
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -934,10 +916,8 @@
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -979,10 +959,8 @@
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1024,10 +1002,8 @@
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1069,10 +1045,8 @@
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1114,10 +1088,8 @@
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1159,10 +1131,8 @@
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1204,10 +1174,8 @@
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1249,10 +1217,8 @@
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1294,10 +1260,8 @@
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1339,10 +1303,8 @@
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1384,10 +1346,8 @@
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1429,10 +1389,8 @@
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1474,10 +1432,8 @@
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1515,10 +1471,8 @@
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1572,10 +1526,8 @@
           <t>0 - 17</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="K25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1586,16 +1538,24 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>لِلَّهِ</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+          <t>لِلهِ</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>asa</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -1606,13 +1566,11 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>10 - 17</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+          <t>12 - 17</t>
+        </is>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1623,16 +1581,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>الْعَالَمِينَ</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+          <t>لِلهِ</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>asa</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
@@ -1643,13 +1609,11 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>24 - 37</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+          <t>12 - 17</t>
+        </is>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1660,17 +1624,29 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>رَبِّ</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+          <t>اِ۬لْحَمْدُ</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>aqaq</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Ar</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>qwqw</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
@@ -1680,13 +1656,11 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>18 - 23</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+          <t>0 - 11</t>
+        </is>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1697,17 +1671,29 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>لِلَّهِ</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
+          <t>اِ۬لْعَٰلَمِينَ</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>aqaq</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Ar</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>qwqw</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
@@ -1717,13 +1703,11 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>10 - 17</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+          <t>24 - 39</t>
+        </is>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1734,17 +1718,29 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>لِلَّهِ رَ</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
+          <t>اِ۬لْعَٰلَمِينَ</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>aqaq</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Ar</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>qwqw</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
@@ -1754,13 +1750,11 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>10 - 20</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+          <t>24 - 39</t>
+        </is>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1771,17 +1765,29 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1:2</t>
+          <t>1:1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>الْحَمْدُ لِلَّهِ</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
+          <t>رَبِّ</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>aqaq</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Ar</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>qwqw</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
@@ -1791,264 +1797,11 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0 - 17</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>1:2</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>الْحَمْدُ</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Konduga</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>0 - 9</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>1:2</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>لِلَّهِ</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Ar</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Mor</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Konduga</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>10 - 17</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>1:2</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>اَ۬لرَّحْمَٰنِ</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Ar</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>tafsir</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>Konduga</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>0 - 14</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>1:1</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>اِ۬لْعَٰلَمِينَ</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Ar</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>tafsir</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>Konduga</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>24 - 39</t>
-        </is>
-      </c>
-      <c r="K35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>1:1</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>لِلهِ</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Ar</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>tafsir</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Konduga</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>12 - 17</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
+          <t>18 - 23</t>
+        </is>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>